<commit_message>
empecé la solución del ejercicio 21 de la sección 2.1
</commit_message>
<xml_diff>
--- a/3_planeacion/2_classes/3_unidad_2_ecuaciones_e_inecuaciones/apendice/ejercicios_colaboracion_equipo/asignacion_ejercicios_cap2.xlsx
+++ b/3_planeacion/2_classes/3_unidad_2_ecuaciones_e_inecuaciones/apendice/ejercicios_colaboracion_equipo/asignacion_ejercicios_cap2.xlsx
@@ -453,7 +453,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Sección 2.4 (Números complejos) - Ejercicio 48, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 43, Sección 2.1 (Ecuaciones) - Ejercicio 51, Sección 2.6 (Desigualdades) - Ejercicio 56, Sección 2.6 (Desigualdades) - Ejercicio 52, Sección 2.1 (Ecuaciones) - Ejercicio 5, Sección 2.2 (Problemas de aplicación) - Ejercicio 12, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 45, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 38, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 13, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 8, Sección 2.4 (Números complejos) - Ejercicio 50, Sección 2.6 (Desigualdades) - Ejercicio 27, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 36, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 33, Sección 2.2 (Problemas de aplicación) - Ejercicio 23, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 25, Sección 2.4 (Números complejos) - Ejercicio 52, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 56, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 21, Sección 2.6 (Desigualdades) - Ejercicio 36, Sección 2.2 (Problemas de aplicación) - Ejercicio 17, Sección 2.2 (Problemas de aplicación) - Ejercicio 38, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 71, Sección 2.6 (Desigualdades) - Ejercicio 5, Sección 2.2 (Problemas de aplicación) - Ejercicio 25</t>
+          <t>Sección 2.1 (Ecuaciones) - Ejercicio 54, Sección 2.4 (Números complejos) - Ejercicio 61, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 71, Sección 2.1 (Ecuaciones) - Ejercicio 51, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 70, Sección 2.6 (Desigualdades) - Ejercicio 17, Sección 2.7 (Valor absoluto) - Ejercicio 35, Sección 2.2 (Problemas de aplicación) - Ejercicio 4, Sección 2.1 (Ecuaciones) - Ejercicio 26, Sección 2.7 (Valor absoluto) - Ejercicio 3, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 56, Sección 2.7 (Valor absoluto) - Ejercicio 19, Sección 2.6 (Desigualdades) - Ejercicio 37, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 63, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 58, Sección 2.6 (Desigualdades) - Ejercicio 28, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 42, Sección 2.1 (Ecuaciones) - Ejercicio 72, Sección 2.6 (Desigualdades) - Ejercicio 46, Sección 2.1 (Ecuaciones) - Ejercicio 71, Sección 2.1 (Ecuaciones) - Ejercicio 74, Sección 2.6 (Desigualdades) - Ejercicio 12, Sección 2.1 (Ecuaciones) - Ejercicio 52, Sección 2.4 (Números complejos) - Ejercicio 45, Sección 2.1 (Ecuaciones) - Ejercicio 64, Sección 2.6 (Desigualdades) - Ejercicio 72</t>
         </is>
       </c>
     </row>
@@ -465,7 +465,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Sección 2.1 (Ecuaciones) - Ejercicio 57, Sección 2.6 (Desigualdades) - Ejercicio 31, Sección 2.7 (Valor absoluto) - Ejercicio 37, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 19, Sección 2.7 (Valor absoluto) - Ejercicio 9, Sección 2.7 (Valor absoluto) - Ejercicio 49, Sección 2.6 (Desigualdades) - Ejercicio 81, Sección 2.1 (Ecuaciones) - Ejercicio 2, Sección 2.7 (Valor absoluto) - Ejercicio 55, Sección 2.1 (Ecuaciones) - Ejercicio 6, Sección 2.1 (Ecuaciones) - Ejercicio 61, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 12, Sección 2.6 (Desigualdades) - Ejercicio 62, Sección 2.4 (Números complejos) - Ejercicio 45, Sección 2.4 (Números complejos) - Ejercicio 21, Sección 2.1 (Ecuaciones) - Ejercicio 33, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 68, Sección 2.1 (Ecuaciones) - Ejercicio 14, Sección 2.1 (Ecuaciones) - Ejercicio 23, Sección 2.6 (Desigualdades) - Ejercicio 9, Sección 2.2 (Problemas de aplicación) - Ejercicio 28, Sección 2.4 (Números complejos) - Ejercicio 62, Sección 2.2 (Problemas de aplicación) - Ejercicio 8, Sección 2.6 (Desigualdades) - Ejercicio 12, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 24, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 69</t>
+          <t>Sección 2.4 (Números complejos) - Ejercicio 23, Sección 2.4 (Números complejos) - Ejercicio 54, Sección 2.4 (Números complejos) - Ejercicio 16, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 10, Sección 2.6 (Desigualdades) - Ejercicio 61, Sección 2.1 (Ecuaciones) - Ejercicio 76, Sección 2.1 (Ecuaciones) - Ejercicio 42, Sección 2.6 (Desigualdades) - Ejercicio 84, Sección 2.6 (Desigualdades) - Ejercicio 53, Sección 2.2 (Problemas de aplicación) - Ejercicio 2, Sección 2.4 (Números complejos) - Ejercicio 13, Sección 2.2 (Problemas de aplicación) - Ejercicio 5, Sección 2.1 (Ecuaciones) - Ejercicio 49, Sección 2.4 (Números complejos) - Ejercicio 35, Sección 2.1 (Ecuaciones) - Ejercicio 78, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 46, Sección 2.1 (Ecuaciones) - Ejercicio 34, Sección 2.4 (Números complejos) - Ejercicio 47, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 48, Sección 2.6 (Desigualdades) - Ejercicio 25, Sección 2.6 (Desigualdades) - Ejercicio 74, Sección 2.2 (Problemas de aplicación) - Ejercicio 20, Sección 2.1 (Ecuaciones) - Ejercicio 70, Sección 2.1 (Ecuaciones) - Ejercicio 24, Sección 2.4 (Números complejos) - Ejercicio 3, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 59</t>
         </is>
       </c>
     </row>
@@ -477,7 +477,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Sección 2.6 (Desigualdades) - Ejercicio 70, Sección 2.6 (Desigualdades) - Ejercicio 46, Sección 2.1 (Ecuaciones) - Ejercicio 8, Sección 2.4 (Números complejos) - Ejercicio 37, Sección 2.7 (Valor absoluto) - Ejercicio 18, Sección 2.1 (Ecuaciones) - Ejercicio 30, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 6, Sección 2.4 (Números complejos) - Ejercicio 23, Sección 2.7 (Valor absoluto) - Ejercicio 48, Sección 2.7 (Valor absoluto) - Ejercicio 28, Sección 2.2 (Problemas de aplicación) - Ejercicio 3, Sección 2.4 (Números complejos) - Ejercicio 56, Sección 2.6 (Desigualdades) - Ejercicio 74, Sección 2.4 (Números complejos) - Ejercicio 35, Sección 2.7 (Valor absoluto) - Ejercicio 25, Sección 2.4 (Números complejos) - Ejercicio 38, Sección 2.1 (Ecuaciones) - Ejercicio 39, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 22, Sección 2.6 (Desigualdades) - Ejercicio 64, Sección 2.7 (Valor absoluto) - Ejercicio 46, Sección 2.7 (Valor absoluto) - Ejercicio 24, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 5, Sección 2.4 (Números complejos) - Ejercicio 58, Sección 2.7 (Valor absoluto) - Ejercicio 29, Sección 2.1 (Ecuaciones) - Ejercicio 43, Sección 2.1 (Ecuaciones) - Ejercicio 49</t>
+          <t>Sección 2.4 (Números complejos) - Ejercicio 12, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 82, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 12, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 53, Sección 2.4 (Números complejos) - Ejercicio 28, Sección 2.2 (Problemas de aplicación) - Ejercicio 3, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 15, Sección 2.1 (Ecuaciones) - Ejercicio 43, Sección 2.7 (Valor absoluto) - Ejercicio 33, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 61, Sección 2.1 (Ecuaciones) - Ejercicio 7, Sección 2.7 (Valor absoluto) - Ejercicio 20, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 16, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 46, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 25, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 39, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 44, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 4, Sección 2.6 (Desigualdades) - Ejercicio 62, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 65, Sección 2.6 (Desigualdades) - Ejercicio 1, Sección 2.2 (Problemas de aplicación) - Ejercicio 13, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 52, Sección 2.7 (Valor absoluto) - Ejercicio 49, Sección 2.6 (Desigualdades) - Ejercicio 80, Sección 2.1 (Ecuaciones) - Ejercicio 1</t>
         </is>
       </c>
     </row>
@@ -489,7 +489,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Sección 2.4 (Números complejos) - Ejercicio 47, Sección 2.6 (Desigualdades) - Ejercicio 40, Sección 2.1 (Ecuaciones) - Ejercicio 69, Sección 2.1 (Ecuaciones) - Ejercicio 76, Sección 2.4 (Números complejos) - Ejercicio 32, Sección 2.1 (Ecuaciones) - Ejercicio 45, Sección 2.4 (Números complejos) - Ejercicio 34, Sección 2.1 (Ecuaciones) - Ejercicio 74, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 55, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 45, Sección 2.1 (Ecuaciones) - Ejercicio 71, Sección 2.6 (Desigualdades) - Ejercicio 24, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 47, Sección 2.6 (Desigualdades) - Ejercicio 11, Sección 2.7 (Valor absoluto) - Ejercicio 20, Sección 2.7 (Valor absoluto) - Ejercicio 38, Sección 2.2 (Problemas de aplicación) - Ejercicio 10, Sección 2.7 (Valor absoluto) - Ejercicio 35, Sección 2.1 (Ecuaciones) - Ejercicio 26, Sección 2.1 (Ecuaciones) - Ejercicio 3, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 39, Sección 2.6 (Desigualdades) - Ejercicio 59, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 7, Sección 2.2 (Problemas de aplicación) - Ejercicio 20, Sección 2.1 (Ecuaciones) - Ejercicio 70</t>
+          <t>Sección 2.6 (Desigualdades) - Ejercicio 52, Sección 2.4 (Números complejos) - Ejercicio 14, Sección 2.4 (Números complejos) - Ejercicio 34, Sección 2.2 (Problemas de aplicación) - Ejercicio 17, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 49, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 34, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 26, Sección 2.2 (Problemas de aplicación) - Ejercicio 23, Sección 2.7 (Valor absoluto) - Ejercicio 34, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 8, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 1, Sección 2.2 (Problemas de aplicación) - Ejercicio 38, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 20, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 20, Sección 2.2 (Problemas de aplicación) - Ejercicio 39, Sección 2.1 (Ecuaciones) - Ejercicio 59, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 53, Sección 2.2 (Problemas de aplicación) - Ejercicio 18, Sección 2.4 (Números complejos) - Ejercicio 2, Sección 2.4 (Números complejos) - Ejercicio 46, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 72, Sección 2.2 (Problemas de aplicación) - Ejercicio 36, Sección 2.1 (Ecuaciones) - Ejercicio 35, Sección 2.4 (Números complejos) - Ejercicio 37, Sección 2.6 (Desigualdades) - Ejercicio 42</t>
         </is>
       </c>
     </row>
@@ -501,7 +501,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Sección 2.4 (Números complejos) - Ejercicio 17, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 18, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 58, Sección 2.4 (Números complejos) - Ejercicio 4, Sección 2.7 (Valor absoluto) - Ejercicio 12, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 56, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 72, Sección 2.1 (Ecuaciones) - Ejercicio 34, Sección 2.6 (Desigualdades) - Ejercicio 7, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 37, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 70, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 23, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 30, Sección 2.6 (Desigualdades) - Ejercicio 66, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 70, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 71, Sección 2.6 (Desigualdades) - Ejercicio 21, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 34, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 66, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 50, Sección 2.7 (Valor absoluto) - Ejercicio 40, Sección 2.6 (Desigualdades) - Ejercicio 29, Sección 2.6 (Desigualdades) - Ejercicio 26, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 32, Sección 2.2 (Problemas de aplicación) - Ejercicio 34</t>
+          <t>Sección 2.1 (Ecuaciones) - Ejercicio 25, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 19, Sección 2.1 (Ecuaciones) - Ejercicio 58, Sección 2.6 (Desigualdades) - Ejercicio 34, Sección 2.1 (Ecuaciones) - Ejercicio 63, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 70, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 11, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 1, Sección 2.6 (Desigualdades) - Ejercicio 7, Sección 2.7 (Valor absoluto) - Ejercicio 54, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 77, Sección 2.1 (Ecuaciones) - Ejercicio 36, Sección 2.7 (Valor absoluto) - Ejercicio 41, Sección 2.7 (Valor absoluto) - Ejercicio 55, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 32, Sección 2.6 (Desigualdades) - Ejercicio 59, Sección 2.1 (Ecuaciones) - Ejercicio 12, Sección 2.7 (Valor absoluto) - Ejercicio 6, Sección 2.4 (Números complejos) - Ejercicio 6, Sección 2.1 (Ecuaciones) - Ejercicio 75, Sección 2.1 (Ecuaciones) - Ejercicio 4, Sección 2.7 (Valor absoluto) - Ejercicio 5, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 24, Sección 2.7 (Valor absoluto) - Ejercicio 23, Sección 2.4 (Números complejos) - Ejercicio 53</t>
         </is>
       </c>
     </row>
@@ -513,7 +513,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Sección 2.6 (Desigualdades) - Ejercicio 42, Sección 2.6 (Desigualdades) - Ejercicio 79, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 49, Sección 2.1 (Ecuaciones) - Ejercicio 24, Sección 2.1 (Ecuaciones) - Ejercicio 48, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 36, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 65, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 11, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 67, Sección 2.1 (Ecuaciones) - Ejercicio 20, Sección 2.6 (Desigualdades) - Ejercicio 16, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 11, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 31, Sección 2.7 (Valor absoluto) - Ejercicio 31, Sección 2.6 (Desigualdades) - Ejercicio 76, Sección 2.1 (Ecuaciones) - Ejercicio 36, Sección 2.4 (Números complejos) - Ejercicio 29, Sección 2.1 (Ecuaciones) - Ejercicio 38, Sección 2.1 (Ecuaciones) - Ejercicio 59, Sección 2.6 (Desigualdades) - Ejercicio 15, Sección 2.1 (Ecuaciones) - Ejercicio 52, Sección 2.4 (Números complejos) - Ejercicio 55, Sección 2.4 (Números complejos) - Ejercicio 30, Sección 2.2 (Problemas de aplicación) - Ejercicio 31, Sección 2.1 (Ecuaciones) - Ejercicio 73</t>
+          <t>Sección 2.6 (Desigualdades) - Ejercicio 50, Sección 2.2 (Problemas de aplicación) - Ejercicio 31, Sección 2.7 (Valor absoluto) - Ejercicio 51, Sección 2.7 (Valor absoluto) - Ejercicio 43, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 66, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 35, Sección 2.2 (Problemas de aplicación) - Ejercicio 16, Sección 2.4 (Números complejos) - Ejercicio 39, Sección 2.6 (Desigualdades) - Ejercicio 15, Sección 2.1 (Ecuaciones) - Ejercicio 60, Sección 2.6 (Desigualdades) - Ejercicio 22, Sección 2.7 (Valor absoluto) - Ejercicio 37, Sección 2.1 (Ecuaciones) - Ejercicio 45, Sección 2.1 (Ecuaciones) - Ejercicio 44, Sección 2.1 (Ecuaciones) - Ejercicio 40, Sección 2.1 (Ecuaciones) - Ejercicio 17, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 51, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 26, Sección 2.4 (Números complejos) - Ejercicio 51, Sección 2.6 (Desigualdades) - Ejercicio 40, Sección 2.2 (Problemas de aplicación) - Ejercicio 6, Sección 2.7 (Valor absoluto) - Ejercicio 2, Sección 2.1 (Ecuaciones) - Ejercicio 15, Sección 2.4 (Números complejos) - Ejercicio 31, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 3</t>
         </is>
       </c>
     </row>
@@ -525,7 +525,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 75, Sección 2.2 (Problemas de aplicación) - Ejercicio 21, Sección 2.6 (Desigualdades) - Ejercicio 53, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 26, Sección 2.7 (Valor absoluto) - Ejercicio 5, Sección 2.7 (Valor absoluto) - Ejercicio 17, Sección 2.1 (Ecuaciones) - Ejercicio 63, Sección 2.6 (Desigualdades) - Ejercicio 39, Sección 2.7 (Valor absoluto) - Ejercicio 6, Sección 2.4 (Números complejos) - Ejercicio 9, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 59, Sección 2.7 (Valor absoluto) - Ejercicio 45, Sección 2.2 (Problemas de aplicación) - Ejercicio 5, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 46, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 30, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 82, Sección 2.7 (Valor absoluto) - Ejercicio 30, Sección 2.7 (Valor absoluto) - Ejercicio 36, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 40, Sección 2.1 (Ecuaciones) - Ejercicio 1, Sección 2.1 (Ecuaciones) - Ejercicio 77, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 62, Sección 2.7 (Valor absoluto) - Ejercicio 8, Sección 2.1 (Ecuaciones) - Ejercicio 19, Sección 2.6 (Desigualdades) - Ejercicio 23</t>
+          <t>Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 56, Sección 2.7 (Valor absoluto) - Ejercicio 36, Sección 2.6 (Desigualdades) - Ejercicio 65, Sección 2.7 (Valor absoluto) - Ejercicio 45, Sección 2.6 (Desigualdades) - Ejercicio 48, Sección 2.6 (Desigualdades) - Ejercicio 21, Sección 2.6 (Desigualdades) - Ejercicio 88, Sección 2.7 (Valor absoluto) - Ejercicio 1, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 27, Sección 2.1 (Ecuaciones) - Ejercicio 9, Sección 2.4 (Números complejos) - Ejercicio 20, Sección 2.4 (Números complejos) - Ejercicio 44, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 69, Sección 2.6 (Desigualdades) - Ejercicio 70, Sección 2.1 (Ecuaciones) - Ejercicio 39, Sección 2.7 (Valor absoluto) - Ejercicio 48, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 10, Sección 2.6 (Desigualdades) - Ejercicio 78, Sección 2.6 (Desigualdades) - Ejercicio 81, Sección 2.1 (Ecuaciones) - Ejercicio 37, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 63, Sección 2.4 (Números complejos) - Ejercicio 1, Sección 2.2 (Problemas de aplicación) - Ejercicio 10, Sección 2.6 (Desigualdades) - Ejercicio 82, Sección 2.4 (Números complejos) - Ejercicio 62</t>
         </is>
       </c>
     </row>
@@ -537,7 +537,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Sección 2.7 (Valor absoluto) - Ejercicio 33, Sección 2.7 (Valor absoluto) - Ejercicio 21, Sección 2.1 (Ecuaciones) - Ejercicio 7, Sección 2.7 (Valor absoluto) - Ejercicio 19, Sección 2.6 (Desigualdades) - Ejercicio 85, Sección 2.4 (Números complejos) - Ejercicio 24, Sección 2.4 (Números complejos) - Ejercicio 42, Sección 2.2 (Problemas de aplicación) - Ejercicio 7, Sección 2.6 (Desigualdades) - Ejercicio 45, Sección 2.7 (Valor absoluto) - Ejercicio 43, Sección 2.7 (Valor absoluto) - Ejercicio 2, Sección 2.6 (Desigualdades) - Ejercicio 75, Sección 2.2 (Problemas de aplicación) - Ejercicio 27, Sección 2.4 (Números complejos) - Ejercicio 13, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 64, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 73, Sección 2.6 (Desigualdades) - Ejercicio 33, Sección 2.6 (Desigualdades) - Ejercicio 80, Sección 2.6 (Desigualdades) - Ejercicio 73, Sección 2.2 (Problemas de aplicación) - Ejercicio 19, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 48, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 37, Sección 2.1 (Ecuaciones) - Ejercicio 44, Sección 2.4 (Números complejos) - Ejercicio 26, Sección 2.7 (Valor absoluto) - Ejercicio 51</t>
+          <t>Sección 2.7 (Valor absoluto) - Ejercicio 12, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 29, Sección 2.6 (Desigualdades) - Ejercicio 63, Sección 2.6 (Desigualdades) - Ejercicio 30, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 9, Sección 2.4 (Números complejos) - Ejercicio 50, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 27, Sección 2.2 (Problemas de aplicación) - Ejercicio 15, Sección 2.7 (Valor absoluto) - Ejercicio 40, Sección 2.6 (Desigualdades) - Ejercicio 4, Sección 2.7 (Valor absoluto) - Ejercicio 26, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 23, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 23, Sección 2.6 (Desigualdades) - Ejercicio 41, Sección 2.4 (Números complejos) - Ejercicio 58, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 5, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 4, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 33, Sección 2.1 (Ecuaciones) - Ejercicio 62, Sección 2.6 (Desigualdades) - Ejercicio 77, Sección 2.6 (Desigualdades) - Ejercicio 56, Sección 2.1 (Ecuaciones) - Ejercicio 47, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 28, Sección 2.4 (Números complejos) - Ejercicio 18, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 17</t>
         </is>
       </c>
     </row>
@@ -549,7 +549,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Sección 2.2 (Problemas de aplicación) - Ejercicio 29, Sección 2.4 (Números complejos) - Ejercicio 18, Sección 2.7 (Valor absoluto) - Ejercicio 44, Sección 2.6 (Desigualdades) - Ejercicio 86, Sección 2.7 (Valor absoluto) - Ejercicio 47, Sección 2.1 (Ecuaciones) - Ejercicio 60, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 19, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 46, Sección 2.1 (Ecuaciones) - Ejercicio 40, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 31, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 54, Sección 2.2 (Problemas de aplicación) - Ejercicio 24, Sección 2.2 (Problemas de aplicación) - Ejercicio 39, Sección 2.6 (Desigualdades) - Ejercicio 47, Sección 2.4 (Números complejos) - Ejercicio 27, Sección 2.2 (Problemas de aplicación) - Ejercicio 16, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 55, Sección 2.4 (Números complejos) - Ejercicio 44, Sección 2.4 (Números complejos) - Ejercicio 22, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 6, Sección 2.7 (Valor absoluto) - Ejercicio 41, Sección 2.2 (Problemas de aplicación) - Ejercicio 33, Sección 2.6 (Desigualdades) - Ejercicio 18, Sección 2.6 (Desigualdades) - Ejercicio 50, Sección 2.6 (Desigualdades) - Ejercicio 87</t>
+          <t>Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 40, Sección 2.6 (Desigualdades) - Ejercicio 26, Sección 2.2 (Problemas de aplicación) - Ejercicio 21, Sección 2.2 (Problemas de aplicación) - Ejercicio 37, Sección 2.2 (Problemas de aplicación) - Ejercicio 27, Sección 2.1 (Ecuaciones) - Ejercicio 29, Sección 2.7 (Valor absoluto) - Ejercicio 18, Sección 2.6 (Desigualdades) - Ejercicio 14, Sección 2.6 (Desigualdades) - Ejercicio 44, Sección 2.4 (Números complejos) - Ejercicio 41, Sección 2.4 (Números complejos) - Ejercicio 30, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 36, Sección 2.6 (Desigualdades) - Ejercicio 47, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 18, Sección 2.1 (Ecuaciones) - Ejercicio 2, Sección 2.6 (Desigualdades) - Ejercicio 89, Sección 2.7 (Valor absoluto) - Ejercicio 22, Sección 2.4 (Números complejos) - Ejercicio 7, Sección 2.1 (Ecuaciones) - Ejercicio 5, Sección 2.4 (Números complejos) - Ejercicio 22, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 35, Sección 2.7 (Valor absoluto) - Ejercicio 53, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 32, Sección 2.1 (Ecuaciones) - Ejercicio 3, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 66</t>
         </is>
       </c>
     </row>
@@ -561,7 +561,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Sección 2.1 (Ecuaciones) - Ejercicio 64, Sección 2.6 (Desigualdades) - Ejercicio 28, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 61, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 40, Sección 2.4 (Números complejos) - Ejercicio 3, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 52, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 8, Sección 2.4 (Números complejos) - Ejercicio 60, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 43, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 14, Sección 2.7 (Valor absoluto) - Ejercicio 13, Sección 2.1 (Ecuaciones) - Ejercicio 4, Sección 2.6 (Desigualdades) - Ejercicio 17, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 81, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 3, Sección 2.6 (Desigualdades) - Ejercicio 58, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 10, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 15, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 53, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 17, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 9, Sección 2.6 (Desigualdades) - Ejercicio 54, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 44, Sección 2.6 (Desigualdades) - Ejercicio 57, Sección 2.6 (Desigualdades) - Ejercicio 67</t>
+          <t>Sección 2.4 (Números complejos) - Ejercicio 8, Sección 2.6 (Desigualdades) - Ejercicio 27, Sección 2.4 (Números complejos) - Ejercicio 5, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 41, Sección 2.7 (Valor absoluto) - Ejercicio 29, Sección 2.1 (Ecuaciones) - Ejercicio 69, Sección 2.7 (Valor absoluto) - Ejercicio 21, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 51, Sección 2.7 (Valor absoluto) - Ejercicio 9, Sección 2.4 (Números complejos) - Ejercicio 15, Sección 2.7 (Valor absoluto) - Ejercicio 24, Sección 2.1 (Ecuaciones) - Ejercicio 21, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 57, Sección 2.1 (Ecuaciones) - Ejercicio 68, Sección 2.6 (Desigualdades) - Ejercicio 58, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 21, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 31, Sección 2.6 (Desigualdades) - Ejercicio 85, Sección 2.7 (Valor absoluto) - Ejercicio 11, Sección 2.4 (Números complejos) - Ejercicio 42, Sección 2.1 (Ecuaciones) - Ejercicio 14, Sección 2.4 (Números complejos) - Ejercicio 49, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 30, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 38, Sección 2.6 (Desigualdades) - Ejercicio 66</t>
         </is>
       </c>
     </row>
@@ -573,7 +573,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Sección 2.1 (Ecuaciones) - Ejercicio 10, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 13, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 28, Sección 2.7 (Valor absoluto) - Ejercicio 1, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 60, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 2, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 12, Sección 2.4 (Números complejos) - Ejercicio 14, Sección 2.4 (Números complejos) - Ejercicio 39, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 20, Sección 2.1 (Ecuaciones) - Ejercicio 18, Sección 2.4 (Números complejos) - Ejercicio 19, Sección 2.4 (Números complejos) - Ejercicio 40, Sección 2.2 (Problemas de aplicación) - Ejercicio 32, Sección 2.1 (Ecuaciones) - Ejercicio 41, Sección 2.1 (Ecuaciones) - Ejercicio 27, Sección 2.4 (Números complejos) - Ejercicio 16, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 68, Sección 2.6 (Desigualdades) - Ejercicio 71, Sección 2.7 (Valor absoluto) - Ejercicio 27, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 78, Sección 2.6 (Desigualdades) - Ejercicio 49, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 4, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 18, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 79</t>
+          <t>Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 80, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 6, Sección 2.7 (Valor absoluto) - Ejercicio 38, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 74, Sección 2.2 (Problemas de aplicación) - Ejercicio 35, Sección 2.1 (Ecuaciones) - Ejercicio 13, Sección 2.1 (Ecuaciones) - Ejercicio 67, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 81, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 67, Sección 2.4 (Números complejos) - Ejercicio 57, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 44, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 43, Sección 2.7 (Valor absoluto) - Ejercicio 17, Sección 2.7 (Valor absoluto) - Ejercicio 8, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 55, Sección 2.2 (Problemas de aplicación) - Ejercicio 28, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 68, Sección 2.2 (Problemas de aplicación) - Ejercicio 34, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 62, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 64, Sección 2.7 (Valor absoluto) - Ejercicio 39, Sección 2.1 (Ecuaciones) - Ejercicio 56, Sección 2.2 (Problemas de aplicación) - Ejercicio 1, Sección 2.6 (Desigualdades) - Ejercicio 54, Sección 2.4 (Números complejos) - Ejercicio 24</t>
         </is>
       </c>
     </row>
@@ -585,7 +585,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 1, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 28, Sección 2.1 (Ecuaciones) - Ejercicio 42, Sección 2.4 (Números complejos) - Ejercicio 28, Sección 2.1 (Ecuaciones) - Ejercicio 56, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 41, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 48, Sección 2.1 (Ecuaciones) - Ejercicio 66, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 7, Sección 2.1 (Ecuaciones) - Ejercicio 50, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 39, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 21, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 10, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 33, Sección 2.4 (Números complejos) - Ejercicio 46, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 20, Sección 2.6 (Desigualdades) - Ejercicio 20, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 32, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 47, Sección 2.7 (Valor absoluto) - Ejercicio 34, Sección 2.1 (Ecuaciones) - Ejercicio 17, Sección 2.4 (Números complejos) - Ejercicio 1, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 23, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 16, Sección 2.7 (Valor absoluto) - Ejercicio 22</t>
+          <t>Sección 2.6 (Desigualdades) - Ejercicio 24, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 39, Sección 2.7 (Valor absoluto) - Ejercicio 16, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 73, Sección 2.4 (Números complejos) - Ejercicio 17, Sección 2.1 (Ecuaciones) - Ejercicio 27, Sección 2.6 (Desigualdades) - Ejercicio 5, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 2, Sección 2.1 (Ecuaciones) - Ejercicio 48, Sección 2.6 (Desigualdades) - Ejercicio 23, Sección 2.2 (Problemas de aplicación) - Ejercicio 9, Sección 2.7 (Valor absoluto) - Ejercicio 10, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 3, Sección 2.2 (Problemas de aplicación) - Ejercicio 32, Sección 2.4 (Números complejos) - Ejercicio 21, Sección 2.6 (Desigualdades) - Ejercicio 71, Sección 2.4 (Números complejos) - Ejercicio 10, Sección 2.1 (Ecuaciones) - Ejercicio 46, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 48, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 47, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 21, Sección 2.1 (Ecuaciones) - Ejercicio 33, Sección 2.4 (Números complejos) - Ejercicio 33, Sección 2.7 (Valor absoluto) - Ejercicio 42, Sección 2.4 (Números complejos) - Ejercicio 40</t>
         </is>
       </c>
     </row>
@@ -597,7 +597,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Sección 2.7 (Valor absoluto) - Ejercicio 52, Sección 2.2 (Problemas de aplicación) - Ejercicio 36, Sección 2.2 (Problemas de aplicación) - Ejercicio 30, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 54, Sección 2.6 (Desigualdades) - Ejercicio 4, Sección 2.2 (Problemas de aplicación) - Ejercicio 6, Sección 2.4 (Números complejos) - Ejercicio 36, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 27, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 66, Sección 2.1 (Ecuaciones) - Ejercicio 68, Sección 2.4 (Números complejos) - Ejercicio 41, Sección 2.6 (Desigualdades) - Ejercicio 63, Sección 2.1 (Ecuaciones) - Ejercicio 16, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 64, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 67, Sección 2.6 (Desigualdades) - Ejercicio 14, Sección 2.6 (Desigualdades) - Ejercicio 35, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 5, Sección 2.4 (Números complejos) - Ejercicio 25, Sección 2.6 (Desigualdades) - Ejercicio 60, Sección 2.1 (Ecuaciones) - Ejercicio 72, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 53, Sección 2.1 (Ecuaciones) - Ejercicio 13, Sección 2.4 (Números complejos) - Ejercicio 57, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 3</t>
+          <t>Sección 2.6 (Desigualdades) - Ejercicio 64, Sección 2.1 (Ecuaciones) - Ejercicio 65, Sección 2.4 (Números complejos) - Ejercicio 36, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 28, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 64, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 31, Sección 2.6 (Desigualdades) - Ejercicio 38, Sección 2.6 (Desigualdades) - Ejercicio 76, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 57, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 37, Sección 2.1 (Ecuaciones) - Ejercicio 57, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 38, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 40, Sección 2.6 (Desigualdades) - Ejercicio 11, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 29, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 25, Sección 2.1 (Ecuaciones) - Ejercicio 32, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 17, Sección 2.1 (Ecuaciones) - Ejercicio 20, Sección 2.2 (Problemas de aplicación) - Ejercicio 26, Sección 2.6 (Desigualdades) - Ejercicio 3, Sección 2.7 (Valor absoluto) - Ejercicio 28, Sección 2.4 (Números complejos) - Ejercicio 43, Sección 2.6 (Desigualdades) - Ejercicio 31, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 59</t>
         </is>
       </c>
     </row>
@@ -609,7 +609,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Sección 2.7 (Valor absoluto) - Ejercicio 16, Sección 2.1 (Ecuaciones) - Ejercicio 22, Sección 2.6 (Desigualdades) - Ejercicio 43, Sección 2.1 (Ecuaciones) - Ejercicio 67, Sección 2.2 (Problemas de aplicación) - Ejercicio 15, Sección 2.6 (Desigualdades) - Ejercicio 84, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 2, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 63, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 50, Sección 2.6 (Desigualdades) - Ejercicio 6, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 52, Sección 2.7 (Valor absoluto) - Ejercicio 7, Sección 2.2 (Problemas de aplicación) - Ejercicio 14, Sección 2.4 (Números complejos) - Ejercicio 43, Sección 2.7 (Valor absoluto) - Ejercicio 4, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 49, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 76, Sección 2.1 (Ecuaciones) - Ejercicio 25, Sección 2.7 (Valor absoluto) - Ejercicio 26, Sección 2.4 (Números complejos) - Ejercicio 15, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 1, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 25, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 59, Sección 2.1 (Ecuaciones) - Ejercicio 78, Sección 2.2 (Problemas de aplicación) - Ejercicio 18</t>
+          <t>Sección 2.1 (Ecuaciones) - Ejercicio 50, Sección 2.6 (Desigualdades) - Ejercicio 86, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 49, Sección 2.4 (Números complejos) - Ejercicio 29, Sección 2.1 (Ecuaciones) - Ejercicio 28, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 5, Sección 2.1 (Ecuaciones) - Ejercicio 6, Sección 2.4 (Números complejos) - Ejercicio 48, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 69, Sección 2.2 (Problemas de aplicación) - Ejercicio 24, Sección 2.1 (Ecuaciones) - Ejercicio 23, Sección 2.6 (Desigualdades) - Ejercicio 83, Sección 2.1 (Ecuaciones) - Ejercicio 11, Sección 2.7 (Valor absoluto) - Ejercicio 52, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 50, Sección 2.1 (Ecuaciones) - Ejercicio 53, Sección 2.6 (Desigualdades) - Ejercicio 36, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 22, Sección 2.6 (Desigualdades) - Ejercicio 20, Sección 2.4 (Números complejos) - Ejercicio 27, Sección 2.6 (Desigualdades) - Ejercicio 49, Sección 2.7 (Valor absoluto) - Ejercicio 44, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 19, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 58, Sección 2.1 (Ecuaciones) - Ejercicio 8</t>
         </is>
       </c>
     </row>
@@ -621,7 +621,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Sección 2.1 (Ecuaciones) - Ejercicio 15, Sección 2.4 (Números complejos) - Ejercicio 2, Sección 2.4 (Números complejos) - Ejercicio 20, Sección 2.6 (Desigualdades) - Ejercicio 25, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 41, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 65, Sección 2.2 (Problemas de aplicación) - Ejercicio 11, Sección 2.6 (Desigualdades) - Ejercicio 10, Sección 2.7 (Valor absoluto) - Ejercicio 53, Sección 2.4 (Números complejos) - Ejercicio 6, Sección 2.4 (Números complejos) - Ejercicio 51, Sección 2.1 (Ecuaciones) - Ejercicio 55, Sección 2.4 (Números complejos) - Ejercicio 7, Sección 2.4 (Números complejos) - Ejercicio 54, Sección 2.4 (Números complejos) - Ejercicio 49, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 44, Sección 2.2 (Problemas de aplicación) - Ejercicio 22, Sección 2.2 (Problemas de aplicación) - Ejercicio 13, Sección 2.2 (Problemas de aplicación) - Ejercicio 9, Sección 2.6 (Desigualdades) - Ejercicio 72, Sección 2.6 (Desigualdades) - Ejercicio 78, Sección 2.6 (Desigualdades) - Ejercicio 83, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 27, Sección 2.1 (Ecuaciones) - Ejercicio 58, Sección 2.6 (Desigualdades) - Ejercicio 41</t>
+          <t>Sección 2.4 (Números complejos) - Ejercicio 56, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 47, Sección 2.2 (Problemas de aplicación) - Ejercicio 30, Sección 2.7 (Valor absoluto) - Ejercicio 7, Sección 2.6 (Desigualdades) - Ejercicio 18, Sección 2.2 (Problemas de aplicación) - Ejercicio 14, Sección 2.6 (Desigualdades) - Ejercicio 10, Sección 2.7 (Valor absoluto) - Ejercicio 30, Sección 2.1 (Ecuaciones) - Ejercicio 18, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 14, Sección 2.6 (Desigualdades) - Ejercicio 13, Sección 2.6 (Desigualdades) - Ejercicio 55, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 71, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 62, Sección 2.7 (Valor absoluto) - Ejercicio 32, Sección 2.7 (Valor absoluto) - Ejercicio 15, Sección 2.1 (Ecuaciones) - Ejercicio 22, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 8, Sección 2.7 (Valor absoluto) - Ejercicio 25, Sección 2.6 (Desigualdades) - Ejercicio 19, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 83, Sección 2.4 (Números complejos) - Ejercicio 38, Sección 2.1 (Ecuaciones) - Ejercicio 16, Sección 2.1 (Ecuaciones) - Ejercicio 41, Sección 2.6 (Desigualdades) - Ejercicio 73</t>
         </is>
       </c>
     </row>
@@ -633,7 +633,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Sección 2.6 (Desigualdades) - Ejercicio 22, Sección 2.1 (Ecuaciones) - Ejercicio 31, Sección 2.1 (Ecuaciones) - Ejercicio 28, Sección 2.6 (Desigualdades) - Ejercicio 89, Sección 2.1 (Ecuaciones) - Ejercicio 47, Sección 2.6 (Desigualdades) - Ejercicio 1, Sección 2.7 (Valor absoluto) - Ejercicio 23, Sección 2.6 (Desigualdades) - Ejercicio 34, Sección 2.6 (Desigualdades) - Ejercicio 44, Sección 2.6 (Desigualdades) - Ejercicio 38, Sección 2.4 (Números complejos) - Ejercicio 8, Sección 2.4 (Números complejos) - Ejercicio 5, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 69, Sección 2.4 (Números complejos) - Ejercicio 31, Sección 2.1 (Ecuaciones) - Ejercicio 32, Sección 2.4 (Números complejos) - Ejercicio 61, Sección 2.6 (Desigualdades) - Ejercicio 82, Sección 2.6 (Desigualdades) - Ejercicio 13, Sección 2.6 (Desigualdades) - Ejercicio 69, Sección 2.1 (Ecuaciones) - Ejercicio 12, Sección 2.1 (Ecuaciones) - Ejercicio 54, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 29, Sección 2.6 (Desigualdades) - Ejercicio 55, Sección 2.2 (Problemas de aplicación) - Ejercicio 2, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 26</t>
+          <t>Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 34, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 41, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 12, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 50, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 54, Sección 2.1 (Ecuaciones) - Ejercicio 31, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 16, Sección 2.4 (Números complejos) - Ejercicio 60, Sección 2.4 (Números complejos) - Ejercicio 25, Sección 2.7 (Valor absoluto) - Ejercicio 13, Sección 2.1 (Ecuaciones) - Ejercicio 10, Sección 2.7 (Valor absoluto) - Ejercicio 14, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 13, Sección 2.4 (Números complejos) - Ejercicio 52, Sección 2.6 (Desigualdades) - Ejercicio 39, Sección 2.2 (Problemas de aplicación) - Ejercicio 8, Sección 2.6 (Desigualdades) - Ejercicio 8, Sección 2.6 (Desigualdades) - Ejercicio 9, Sección 2.6 (Desigualdades) - Ejercicio 57, Sección 2.4 (Números complejos) - Ejercicio 19, Sección 2.2 (Problemas de aplicación) - Ejercicio 40, Sección 2.6 (Desigualdades) - Ejercicio 2, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 14, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 43, Sección 2.6 (Desigualdades) - Ejercicio 35</t>
         </is>
       </c>
     </row>
@@ -645,7 +645,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Sección 2.1 (Ecuaciones) - Ejercicio 75, Sección 2.1 (Ecuaciones) - Ejercicio 46, Sección 2.4 (Números complejos) - Ejercicio 11, Sección 2.6 (Desigualdades) - Ejercicio 32, Sección 2.2 (Problemas de aplicación) - Ejercicio 35, Sección 2.7 (Valor absoluto) - Ejercicio 11, Sección 2.6 (Desigualdades) - Ejercicio 30, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 4, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 14, Sección 2.7 (Valor absoluto) - Ejercicio 39, Sección 2.2 (Problemas de aplicación) - Ejercicio 1, Sección 2.1 (Ecuaciones) - Ejercicio 53, Sección 2.7 (Valor absoluto) - Ejercicio 54, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 77, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 51, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 35, Sección 2.4 (Números complejos) - Ejercicio 59, Sección 2.4 (Números complejos) - Ejercicio 12, Sección 2.6 (Desigualdades) - Ejercicio 77, Sección 2.7 (Valor absoluto) - Ejercicio 42, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 57, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 17, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 83, Sección 2.7 (Valor absoluto) - Ejercicio 32, Sección 2.7 (Valor absoluto) - Ejercicio 15</t>
+          <t>Sección 2.6 (Desigualdades) - Ejercicio 43, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 60, Sección 2.7 (Valor absoluto) - Ejercicio 50, Sección 2.1 (Ecuaciones) - Ejercicio 73, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 54, Sección 2.2 (Problemas de aplicación) - Ejercicio 22, Sección 2.6 (Desigualdades) - Ejercicio 87, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 11, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 75, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 76, Sección 2.7 (Valor absoluto) - Ejercicio 4, Sección 2.4 (Números complejos) - Ejercicio 9, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 79, Sección 2.1 (Ecuaciones) - Ejercicio 55, Sección 2.2 (Problemas de aplicación) - Ejercicio 11, Sección 2.7 (Valor absoluto) - Ejercicio 31, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 42, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 45, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 68, Sección 2.2 (Problemas de aplicación) - Ejercicio 29, Sección 2.6 (Desigualdades) - Ejercicio 75, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 52, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 45, Sección 2.4 (Números complejos) - Ejercicio 32, Sección 2.7 (Valor absoluto) - Ejercicio 27</t>
         </is>
       </c>
     </row>
@@ -657,7 +657,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Sección 2.1 (Ecuaciones) - Ejercicio 37, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 42, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 60, Sección 2.1 (Ecuaciones) - Ejercicio 62, Sección 2.6 (Desigualdades) - Ejercicio 3, Sección 2.2 (Problemas de aplicación) - Ejercicio 26, Sección 2.1 (Ecuaciones) - Ejercicio 29, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 74, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 58, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 80, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 35, Sección 2.4 (Números complejos) - Ejercicio 53, Sección 2.7 (Valor absoluto) - Ejercicio 14, Sección 2.6 (Desigualdades) - Ejercicio 65, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 62, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 38, Sección 2.2 (Problemas de aplicación) - Ejercicio 37, Sección 2.7 (Valor absoluto) - Ejercicio 10, Sección 2.6 (Desigualdades) - Ejercicio 61, Sección 2.7 (Valor absoluto) - Ejercicio 3, Sección 2.6 (Desigualdades) - Ejercicio 8, Sección 2.6 (Desigualdades) - Ejercicio 51, Sección 2.6 (Desigualdades) - Ejercicio 19, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 57, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 9</t>
+          <t>Sección 2.2 (Problemas de aplicación) - Ejercicio 7, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 61, Sección 2.6 (Desigualdades) - Ejercicio 60, Sección 2.2 (Problemas de aplicación) - Ejercicio 33, Sección 2.4 (Números complejos) - Ejercicio 4, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 9, Sección 2.6 (Desigualdades) - Ejercicio 32, Sección 2.6 (Desigualdades) - Ejercicio 68, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 33, Sección 2.4 (Números complejos) - Ejercicio 11, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 78, Sección 2.6 (Desigualdades) - Ejercicio 51, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 65, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 6, Sección 2.1 (Ecuaciones) - Ejercicio 30, Sección 2.6 (Desigualdades) - Ejercicio 45, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 13, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 7, Sección 2.6 (Desigualdades) - Ejercicio 33, Sección 2.1 (Ecuaciones) - Ejercicio 38, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 15, Sección 2.6 (Desigualdades) - Ejercicio 67, Sección 2.6 (Desigualdades) - Ejercicio 69, Sección 2.2 (Problemas de aplicación) - Ejercicio 19, Sección 2.6 (Desigualdades) - Ejercicio 16</t>
         </is>
       </c>
     </row>
@@ -669,7 +669,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Sección 2.1 (Ecuaciones) - Ejercicio 21, Sección 2.1 (Ecuaciones) - Ejercicio 35, Sección 2.6 (Desigualdades) - Ejercicio 68, Sección 2.6 (Desigualdades) - Ejercicio 2, Sección 2.6 (Desigualdades) - Ejercicio 37, Sección 2.2 (Problemas de aplicación) - Ejercicio 4, Sección 2.7 (Valor absoluto) - Ejercicio 50, Sección 2.6 (Desigualdades) - Ejercicio 48, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 51, Sección 2.2 (Problemas de aplicación) - Ejercicio 40, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 42, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 61, Sección 2.1 (Ecuaciones) - Ejercicio 9, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 22, Sección 2.1 (Ecuaciones) - Ejercicio 11, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 29, Sección 2.6 (Desigualdades) - Ejercicio 88, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 24, Sección 2.4 (Números complejos) - Ejercicio 33, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 16, Sección 2.1 (Ecuaciones) - Ejercicio 65, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 34, Sección 2.4 (Números complejos) - Ejercicio 10, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 15, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 63</t>
+          <t>Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 18, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 37, Sección 2.2 (Problemas de aplicación) - Ejercicio 12, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 2, Sección 2.1 (Ecuaciones) - Ejercicio 66, Sección 2.4 (Números complejos) - Ejercicio 59, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 30, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 60, Sección 2.6 (Desigualdades) - Ejercicio 29, Sección 2.7 (Valor absoluto) - Ejercicio 47, Sección 2.2 (Problemas de aplicación) - Ejercicio 25, Sección 2.4 (Números complejos) - Ejercicio 26, Sección 2.1 (Ecuaciones) - Ejercicio 77, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 55, Sección 2.6 (Desigualdades) - Ejercicio 79, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 67, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 22, Sección 2.1 (Ecuaciones) - Ejercicio 61, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 24, Sección 2.6 (Desigualdades) - Ejercicio 6, Sección 2.4 (Números complejos) - Ejercicio 55, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 36, Sección 2.1 (Ecuaciones) - Ejercicio 19, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 7, Sección 2.7 (Valor absoluto) - Ejercicio 46</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Ya empecé a realizar mi segundo ejercicio ilustrativo
</commit_message>
<xml_diff>
--- a/3_planeacion/2_classes/3_unidad_2_ecuaciones_e_inecuaciones/apendice/ejercicios_colaboracion_equipo/asignacion_ejercicios_cap2.xlsx
+++ b/3_planeacion/2_classes/3_unidad_2_ecuaciones_e_inecuaciones/apendice/ejercicios_colaboracion_equipo/asignacion_ejercicios_cap2.xlsx
@@ -453,7 +453,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Sección 2.1 (Ecuaciones) - Ejercicio 54, Sección 2.4 (Números complejos) - Ejercicio 61, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 71, Sección 2.1 (Ecuaciones) - Ejercicio 51, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 70, Sección 2.6 (Desigualdades) - Ejercicio 17, Sección 2.7 (Valor absoluto) - Ejercicio 35, Sección 2.2 (Problemas de aplicación) - Ejercicio 4, Sección 2.1 (Ecuaciones) - Ejercicio 26, Sección 2.7 (Valor absoluto) - Ejercicio 3, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 56, Sección 2.7 (Valor absoluto) - Ejercicio 19, Sección 2.6 (Desigualdades) - Ejercicio 37, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 63, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 58, Sección 2.6 (Desigualdades) - Ejercicio 28, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 42, Sección 2.1 (Ecuaciones) - Ejercicio 72, Sección 2.6 (Desigualdades) - Ejercicio 46, Sección 2.1 (Ecuaciones) - Ejercicio 71, Sección 2.1 (Ecuaciones) - Ejercicio 74, Sección 2.6 (Desigualdades) - Ejercicio 12, Sección 2.1 (Ecuaciones) - Ejercicio 52, Sección 2.4 (Números complejos) - Ejercicio 45, Sección 2.1 (Ecuaciones) - Ejercicio 64, Sección 2.6 (Desigualdades) - Ejercicio 72</t>
+          <t>Sección 2.7 (Valor absoluto) - Ejercicio 44, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 59, Sección 2.6 (Desigualdades) - Ejercicio 23, Sección 2.2 (Problemas de aplicación) - Ejercicio 25, Sección 2.6 (Desigualdades) - Ejercicio 83, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 36, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 73, Sección 2.7 (Valor absoluto) - Ejercicio 37, Sección 2.6 (Desigualdades) - Ejercicio 59, Sección 2.1 (Ecuaciones) - Ejercicio 21, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 23, Sección 2.4 (Números complejos) - Ejercicio 54, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 68, Sección 2.1 (Ecuaciones) - Ejercicio 41, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 71, Sección 2.2 (Problemas de aplicación) - Ejercicio 37, Sección 2.7 (Valor absoluto) - Ejercicio 12, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 50, Sección 2.1 (Ecuaciones) - Ejercicio 26, Sección 2.7 (Valor absoluto) - Ejercicio 48, Sección 2.2 (Problemas de aplicación) - Ejercicio 13, Sección 2.7 (Valor absoluto) - Ejercicio 27, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 69, Sección 2.4 (Números complejos) - Ejercicio 3, Sección 2.1 (Ecuaciones) - Ejercicio 16, Sección 2.4 (Números complejos) - Ejercicio 33</t>
         </is>
       </c>
     </row>
@@ -465,7 +465,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Sección 2.4 (Números complejos) - Ejercicio 23, Sección 2.4 (Números complejos) - Ejercicio 54, Sección 2.4 (Números complejos) - Ejercicio 16, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 10, Sección 2.6 (Desigualdades) - Ejercicio 61, Sección 2.1 (Ecuaciones) - Ejercicio 76, Sección 2.1 (Ecuaciones) - Ejercicio 42, Sección 2.6 (Desigualdades) - Ejercicio 84, Sección 2.6 (Desigualdades) - Ejercicio 53, Sección 2.2 (Problemas de aplicación) - Ejercicio 2, Sección 2.4 (Números complejos) - Ejercicio 13, Sección 2.2 (Problemas de aplicación) - Ejercicio 5, Sección 2.1 (Ecuaciones) - Ejercicio 49, Sección 2.4 (Números complejos) - Ejercicio 35, Sección 2.1 (Ecuaciones) - Ejercicio 78, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 46, Sección 2.1 (Ecuaciones) - Ejercicio 34, Sección 2.4 (Números complejos) - Ejercicio 47, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 48, Sección 2.6 (Desigualdades) - Ejercicio 25, Sección 2.6 (Desigualdades) - Ejercicio 74, Sección 2.2 (Problemas de aplicación) - Ejercicio 20, Sección 2.1 (Ecuaciones) - Ejercicio 70, Sección 2.1 (Ecuaciones) - Ejercicio 24, Sección 2.4 (Números complejos) - Ejercicio 3, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 59</t>
+          <t>Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 63, Sección 2.4 (Números complejos) - Ejercicio 42, Sección 2.6 (Desigualdades) - Ejercicio 20, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 7, Sección 2.2 (Problemas de aplicación) - Ejercicio 5, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 30, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 60, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 52, Sección 2.1 (Ecuaciones) - Ejercicio 18, Sección 2.2 (Problemas de aplicación) - Ejercicio 6, Sección 2.1 (Ecuaciones) - Ejercicio 1, Sección 2.1 (Ecuaciones) - Ejercicio 66, Sección 2.1 (Ecuaciones) - Ejercicio 22, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 2, Sección 2.6 (Desigualdades) - Ejercicio 43, Sección 2.6 (Desigualdades) - Ejercicio 39, Sección 2.7 (Valor absoluto) - Ejercicio 3, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 51, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 72, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 4, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 40, Sección 2.6 (Desigualdades) - Ejercicio 10, Sección 2.7 (Valor absoluto) - Ejercicio 15, Sección 2.6 (Desigualdades) - Ejercicio 27, Sección 2.2 (Problemas de aplicación) - Ejercicio 19, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 39</t>
         </is>
       </c>
     </row>
@@ -477,7 +477,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Sección 2.4 (Números complejos) - Ejercicio 12, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 82, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 12, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 53, Sección 2.4 (Números complejos) - Ejercicio 28, Sección 2.2 (Problemas de aplicación) - Ejercicio 3, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 15, Sección 2.1 (Ecuaciones) - Ejercicio 43, Sección 2.7 (Valor absoluto) - Ejercicio 33, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 61, Sección 2.1 (Ecuaciones) - Ejercicio 7, Sección 2.7 (Valor absoluto) - Ejercicio 20, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 16, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 46, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 25, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 39, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 44, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 4, Sección 2.6 (Desigualdades) - Ejercicio 62, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 65, Sección 2.6 (Desigualdades) - Ejercicio 1, Sección 2.2 (Problemas de aplicación) - Ejercicio 13, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 52, Sección 2.7 (Valor absoluto) - Ejercicio 49, Sección 2.6 (Desigualdades) - Ejercicio 80, Sección 2.1 (Ecuaciones) - Ejercicio 1</t>
+          <t>Sección 2.2 (Problemas de aplicación) - Ejercicio 21, Sección 2.1 (Ecuaciones) - Ejercicio 25, Sección 2.4 (Números complejos) - Ejercicio 2, Sección 2.2 (Problemas de aplicación) - Ejercicio 14, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 16, Sección 2.1 (Ecuaciones) - Ejercicio 27, Sección 2.7 (Valor absoluto) - Ejercicio 32, Sección 2.6 (Desigualdades) - Ejercicio 40, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 79, Sección 2.7 (Valor absoluto) - Ejercicio 29, Sección 2.6 (Desigualdades) - Ejercicio 70, Sección 2.4 (Números complejos) - Ejercicio 49, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 11, Sección 2.6 (Desigualdades) - Ejercicio 5, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 13, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 32, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 8, Sección 2.7 (Valor absoluto) - Ejercicio 18, Sección 2.6 (Desigualdades) - Ejercicio 19, Sección 2.2 (Problemas de aplicación) - Ejercicio 20, Sección 2.7 (Valor absoluto) - Ejercicio 14, Sección 2.4 (Números complejos) - Ejercicio 61, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 41, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 26, Sección 2.1 (Ecuaciones) - Ejercicio 28, Sección 2.1 (Ecuaciones) - Ejercicio 40</t>
         </is>
       </c>
     </row>
@@ -489,7 +489,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Sección 2.6 (Desigualdades) - Ejercicio 52, Sección 2.4 (Números complejos) - Ejercicio 14, Sección 2.4 (Números complejos) - Ejercicio 34, Sección 2.2 (Problemas de aplicación) - Ejercicio 17, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 49, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 34, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 26, Sección 2.2 (Problemas de aplicación) - Ejercicio 23, Sección 2.7 (Valor absoluto) - Ejercicio 34, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 8, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 1, Sección 2.2 (Problemas de aplicación) - Ejercicio 38, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 20, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 20, Sección 2.2 (Problemas de aplicación) - Ejercicio 39, Sección 2.1 (Ecuaciones) - Ejercicio 59, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 53, Sección 2.2 (Problemas de aplicación) - Ejercicio 18, Sección 2.4 (Números complejos) - Ejercicio 2, Sección 2.4 (Números complejos) - Ejercicio 46, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 72, Sección 2.2 (Problemas de aplicación) - Ejercicio 36, Sección 2.1 (Ecuaciones) - Ejercicio 35, Sección 2.4 (Números complejos) - Ejercicio 37, Sección 2.6 (Desigualdades) - Ejercicio 42</t>
+          <t>Sección 2.6 (Desigualdades) - Ejercicio 34, Sección 2.6 (Desigualdades) - Ejercicio 7, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 1, Sección 2.6 (Desigualdades) - Ejercicio 17, Sección 2.1 (Ecuaciones) - Ejercicio 65, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 33, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 29, Sección 2.6 (Desigualdades) - Ejercicio 52, Sección 2.6 (Desigualdades) - Ejercicio 86, Sección 2.1 (Ecuaciones) - Ejercicio 17, Sección 2.6 (Desigualdades) - Ejercicio 22, Sección 2.4 (Números complejos) - Ejercicio 6, Sección 2.6 (Desigualdades) - Ejercicio 35, Sección 2.4 (Números complejos) - Ejercicio 10, Sección 2.1 (Ecuaciones) - Ejercicio 71, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 48, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 44, Sección 2.1 (Ecuaciones) - Ejercicio 35, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 5, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 26, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 76, Sección 2.6 (Desigualdades) - Ejercicio 38, Sección 2.4 (Números complejos) - Ejercicio 14, Sección 2.2 (Problemas de aplicación) - Ejercicio 38, Sección 2.1 (Ecuaciones) - Ejercicio 62</t>
         </is>
       </c>
     </row>
@@ -501,7 +501,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Sección 2.1 (Ecuaciones) - Ejercicio 25, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 19, Sección 2.1 (Ecuaciones) - Ejercicio 58, Sección 2.6 (Desigualdades) - Ejercicio 34, Sección 2.1 (Ecuaciones) - Ejercicio 63, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 70, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 11, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 1, Sección 2.6 (Desigualdades) - Ejercicio 7, Sección 2.7 (Valor absoluto) - Ejercicio 54, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 77, Sección 2.1 (Ecuaciones) - Ejercicio 36, Sección 2.7 (Valor absoluto) - Ejercicio 41, Sección 2.7 (Valor absoluto) - Ejercicio 55, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 32, Sección 2.6 (Desigualdades) - Ejercicio 59, Sección 2.1 (Ecuaciones) - Ejercicio 12, Sección 2.7 (Valor absoluto) - Ejercicio 6, Sección 2.4 (Números complejos) - Ejercicio 6, Sección 2.1 (Ecuaciones) - Ejercicio 75, Sección 2.1 (Ecuaciones) - Ejercicio 4, Sección 2.7 (Valor absoluto) - Ejercicio 5, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 24, Sección 2.7 (Valor absoluto) - Ejercicio 23, Sección 2.4 (Números complejos) - Ejercicio 53</t>
+          <t>Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 66, Sección 2.6 (Desigualdades) - Ejercicio 2, Sección 2.7 (Valor absoluto) - Ejercicio 8, Sección 2.6 (Desigualdades) - Ejercicio 26, Sección 2.4 (Números complejos) - Ejercicio 7, Sección 2.1 (Ecuaciones) - Ejercicio 2, Sección 2.6 (Desigualdades) - Ejercicio 11, Sección 2.7 (Valor absoluto) - Ejercicio 16, Sección 2.4 (Números complejos) - Ejercicio 11, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 22, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 80, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 61, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 82, Sección 2.1 (Ecuaciones) - Ejercicio 74, Sección 2.6 (Desigualdades) - Ejercicio 65, Sección 2.6 (Desigualdades) - Ejercicio 1, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 77, Sección 2.7 (Valor absoluto) - Ejercicio 13, Sección 2.7 (Valor absoluto) - Ejercicio 47, Sección 2.1 (Ecuaciones) - Ejercicio 23, Sección 2.4 (Números complejos) - Ejercicio 38, Sección 2.6 (Desigualdades) - Ejercicio 72, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 12, Sección 2.7 (Valor absoluto) - Ejercicio 2, Sección 2.6 (Desigualdades) - Ejercicio 42</t>
         </is>
       </c>
     </row>
@@ -513,7 +513,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Sección 2.6 (Desigualdades) - Ejercicio 50, Sección 2.2 (Problemas de aplicación) - Ejercicio 31, Sección 2.7 (Valor absoluto) - Ejercicio 51, Sección 2.7 (Valor absoluto) - Ejercicio 43, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 66, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 35, Sección 2.2 (Problemas de aplicación) - Ejercicio 16, Sección 2.4 (Números complejos) - Ejercicio 39, Sección 2.6 (Desigualdades) - Ejercicio 15, Sección 2.1 (Ecuaciones) - Ejercicio 60, Sección 2.6 (Desigualdades) - Ejercicio 22, Sección 2.7 (Valor absoluto) - Ejercicio 37, Sección 2.1 (Ecuaciones) - Ejercicio 45, Sección 2.1 (Ecuaciones) - Ejercicio 44, Sección 2.1 (Ecuaciones) - Ejercicio 40, Sección 2.1 (Ecuaciones) - Ejercicio 17, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 51, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 26, Sección 2.4 (Números complejos) - Ejercicio 51, Sección 2.6 (Desigualdades) - Ejercicio 40, Sección 2.2 (Problemas de aplicación) - Ejercicio 6, Sección 2.7 (Valor absoluto) - Ejercicio 2, Sección 2.1 (Ecuaciones) - Ejercicio 15, Sección 2.4 (Números complejos) - Ejercicio 31, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 3</t>
+          <t>Sección 2.6 (Desigualdades) - Ejercicio 49, Sección 2.4 (Números complejos) - Ejercicio 16, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 12, Sección 2.1 (Ecuaciones) - Ejercicio 36, Sección 2.7 (Valor absoluto) - Ejercicio 26, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 13, Sección 2.7 (Valor absoluto) - Ejercicio 5, Sección 2.4 (Números complejos) - Ejercicio 55, Sección 2.6 (Desigualdades) - Ejercicio 46, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 74, Sección 2.4 (Números complejos) - Ejercicio 46, Sección 2.7 (Valor absoluto) - Ejercicio 31, Sección 2.6 (Desigualdades) - Ejercicio 44, Sección 2.6 (Desigualdades) - Ejercicio 54, Sección 2.4 (Números complejos) - Ejercicio 25, Sección 2.1 (Ecuaciones) - Ejercicio 56, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 6, Sección 2.1 (Ecuaciones) - Ejercicio 6, Sección 2.6 (Desigualdades) - Ejercicio 47, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 33, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 25, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 56, Sección 2.6 (Desigualdades) - Ejercicio 12, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 42, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 15</t>
         </is>
       </c>
     </row>
@@ -525,7 +525,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 56, Sección 2.7 (Valor absoluto) - Ejercicio 36, Sección 2.6 (Desigualdades) - Ejercicio 65, Sección 2.7 (Valor absoluto) - Ejercicio 45, Sección 2.6 (Desigualdades) - Ejercicio 48, Sección 2.6 (Desigualdades) - Ejercicio 21, Sección 2.6 (Desigualdades) - Ejercicio 88, Sección 2.7 (Valor absoluto) - Ejercicio 1, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 27, Sección 2.1 (Ecuaciones) - Ejercicio 9, Sección 2.4 (Números complejos) - Ejercicio 20, Sección 2.4 (Números complejos) - Ejercicio 44, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 69, Sección 2.6 (Desigualdades) - Ejercicio 70, Sección 2.1 (Ecuaciones) - Ejercicio 39, Sección 2.7 (Valor absoluto) - Ejercicio 48, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 10, Sección 2.6 (Desigualdades) - Ejercicio 78, Sección 2.6 (Desigualdades) - Ejercicio 81, Sección 2.1 (Ecuaciones) - Ejercicio 37, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 63, Sección 2.4 (Números complejos) - Ejercicio 1, Sección 2.2 (Problemas de aplicación) - Ejercicio 10, Sección 2.6 (Desigualdades) - Ejercicio 82, Sección 2.4 (Números complejos) - Ejercicio 62</t>
+          <t>Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 62, Sección 2.6 (Desigualdades) - Ejercicio 77, Sección 2.1 (Ecuaciones) - Ejercicio 52, Sección 2.2 (Problemas de aplicación) - Ejercicio 3, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 67, Sección 2.1 (Ecuaciones) - Ejercicio 57, Sección 2.2 (Problemas de aplicación) - Ejercicio 33, Sección 2.1 (Ecuaciones) - Ejercicio 3, Sección 2.7 (Valor absoluto) - Ejercicio 55, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 34, Sección 2.1 (Ecuaciones) - Ejercicio 33, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 38, Sección 2.6 (Desigualdades) - Ejercicio 78, Sección 2.7 (Valor absoluto) - Ejercicio 40, Sección 2.2 (Problemas de aplicación) - Ejercicio 35, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 57, Sección 2.6 (Desigualdades) - Ejercicio 69, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 6, Sección 2.6 (Desigualdades) - Ejercicio 81, Sección 2.6 (Desigualdades) - Ejercicio 31, Sección 2.4 (Números complejos) - Ejercicio 1, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 40, Sección 2.1 (Ecuaciones) - Ejercicio 50, Sección 2.4 (Números complejos) - Ejercicio 17, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 44</t>
         </is>
       </c>
     </row>
@@ -537,7 +537,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Sección 2.7 (Valor absoluto) - Ejercicio 12, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 29, Sección 2.6 (Desigualdades) - Ejercicio 63, Sección 2.6 (Desigualdades) - Ejercicio 30, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 9, Sección 2.4 (Números complejos) - Ejercicio 50, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 27, Sección 2.2 (Problemas de aplicación) - Ejercicio 15, Sección 2.7 (Valor absoluto) - Ejercicio 40, Sección 2.6 (Desigualdades) - Ejercicio 4, Sección 2.7 (Valor absoluto) - Ejercicio 26, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 23, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 23, Sección 2.6 (Desigualdades) - Ejercicio 41, Sección 2.4 (Números complejos) - Ejercicio 58, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 5, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 4, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 33, Sección 2.1 (Ecuaciones) - Ejercicio 62, Sección 2.6 (Desigualdades) - Ejercicio 77, Sección 2.6 (Desigualdades) - Ejercicio 56, Sección 2.1 (Ecuaciones) - Ejercicio 47, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 28, Sección 2.4 (Números complejos) - Ejercicio 18, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 17</t>
+          <t>Sección 2.7 (Valor absoluto) - Ejercicio 6, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 23, Sección 2.2 (Problemas de aplicación) - Ejercicio 29, Sección 2.4 (Números complejos) - Ejercicio 21, Sección 2.1 (Ecuaciones) - Ejercicio 13, Sección 2.6 (Desigualdades) - Ejercicio 75, Sección 2.4 (Números complejos) - Ejercicio 5, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 3, Sección 2.7 (Valor absoluto) - Ejercicio 45, Sección 2.6 (Desigualdades) - Ejercicio 25, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 63, Sección 2.6 (Desigualdades) - Ejercicio 29, Sección 2.2 (Problemas de aplicación) - Ejercicio 22, Sección 2.6 (Desigualdades) - Ejercicio 71, Sección 2.7 (Valor absoluto) - Ejercicio 24, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 75, Sección 2.2 (Problemas de aplicación) - Ejercicio 11, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 17, Sección 2.6 (Desigualdades) - Ejercicio 24, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 58, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 2, Sección 2.2 (Problemas de aplicación) - Ejercicio 36, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 21, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 1, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 46</t>
         </is>
       </c>
     </row>
@@ -549,7 +549,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 40, Sección 2.6 (Desigualdades) - Ejercicio 26, Sección 2.2 (Problemas de aplicación) - Ejercicio 21, Sección 2.2 (Problemas de aplicación) - Ejercicio 37, Sección 2.2 (Problemas de aplicación) - Ejercicio 27, Sección 2.1 (Ecuaciones) - Ejercicio 29, Sección 2.7 (Valor absoluto) - Ejercicio 18, Sección 2.6 (Desigualdades) - Ejercicio 14, Sección 2.6 (Desigualdades) - Ejercicio 44, Sección 2.4 (Números complejos) - Ejercicio 41, Sección 2.4 (Números complejos) - Ejercicio 30, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 36, Sección 2.6 (Desigualdades) - Ejercicio 47, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 18, Sección 2.1 (Ecuaciones) - Ejercicio 2, Sección 2.6 (Desigualdades) - Ejercicio 89, Sección 2.7 (Valor absoluto) - Ejercicio 22, Sección 2.4 (Números complejos) - Ejercicio 7, Sección 2.1 (Ecuaciones) - Ejercicio 5, Sección 2.4 (Números complejos) - Ejercicio 22, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 35, Sección 2.7 (Valor absoluto) - Ejercicio 53, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 32, Sección 2.1 (Ecuaciones) - Ejercicio 3, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 66</t>
+          <t>Sección 2.4 (Números complejos) - Ejercicio 36, Sección 2.7 (Valor absoluto) - Ejercicio 50, Sección 2.6 (Desigualdades) - Ejercicio 74, Sección 2.7 (Valor absoluto) - Ejercicio 21, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 52, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 65, Sección 2.2 (Problemas de aplicación) - Ejercicio 8, Sección 2.6 (Desigualdades) - Ejercicio 63, Sección 2.4 (Números complejos) - Ejercicio 56, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 58, Sección 2.6 (Desigualdades) - Ejercicio 62, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 49, Sección 2.7 (Valor absoluto) - Ejercicio 22, Sección 2.2 (Problemas de aplicación) - Ejercicio 9, Sección 2.1 (Ecuaciones) - Ejercicio 4, Sección 2.7 (Valor absoluto) - Ejercicio 49, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 10, Sección 2.7 (Valor absoluto) - Ejercicio 38, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 43, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 17, Sección 2.4 (Números complejos) - Ejercicio 34, Sección 2.6 (Desigualdades) - Ejercicio 37, Sección 2.1 (Ecuaciones) - Ejercicio 44, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 16, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 39</t>
         </is>
       </c>
     </row>
@@ -561,7 +561,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Sección 2.4 (Números complejos) - Ejercicio 8, Sección 2.6 (Desigualdades) - Ejercicio 27, Sección 2.4 (Números complejos) - Ejercicio 5, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 41, Sección 2.7 (Valor absoluto) - Ejercicio 29, Sección 2.1 (Ecuaciones) - Ejercicio 69, Sección 2.7 (Valor absoluto) - Ejercicio 21, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 51, Sección 2.7 (Valor absoluto) - Ejercicio 9, Sección 2.4 (Números complejos) - Ejercicio 15, Sección 2.7 (Valor absoluto) - Ejercicio 24, Sección 2.1 (Ecuaciones) - Ejercicio 21, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 57, Sección 2.1 (Ecuaciones) - Ejercicio 68, Sección 2.6 (Desigualdades) - Ejercicio 58, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 21, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 31, Sección 2.6 (Desigualdades) - Ejercicio 85, Sección 2.7 (Valor absoluto) - Ejercicio 11, Sección 2.4 (Números complejos) - Ejercicio 42, Sección 2.1 (Ecuaciones) - Ejercicio 14, Sección 2.4 (Números complejos) - Ejercicio 49, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 30, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 38, Sección 2.6 (Desigualdades) - Ejercicio 66</t>
+          <t>Sección 2.6 (Desigualdades) - Ejercicio 73, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 70, Sección 2.2 (Problemas de aplicación) - Ejercicio 1, Sección 2.6 (Desigualdades) - Ejercicio 60, Sección 2.6 (Desigualdades) - Ejercicio 50, Sección 2.4 (Números complejos) - Ejercicio 26, Sección 2.2 (Problemas de aplicación) - Ejercicio 17, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 41, Sección 2.6 (Desigualdades) - Ejercicio 80, Sección 2.1 (Ecuaciones) - Ejercicio 77, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 28, Sección 2.6 (Desigualdades) - Ejercicio 82, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 11, Sección 2.4 (Números complejos) - Ejercicio 15, Sección 2.4 (Números complejos) - Ejercicio 59, Sección 2.2 (Problemas de aplicación) - Ejercicio 2, Sección 2.6 (Desigualdades) - Ejercicio 13, Sección 2.4 (Números complejos) - Ejercicio 18, Sección 2.4 (Números complejos) - Ejercicio 22, Sección 2.2 (Problemas de aplicación) - Ejercicio 27, Sección 2.4 (Números complejos) - Ejercicio 40, Sección 2.6 (Desigualdades) - Ejercicio 85, Sección 2.4 (Números complejos) - Ejercicio 20, Sección 2.2 (Problemas de aplicación) - Ejercicio 30, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 36</t>
         </is>
       </c>
     </row>
@@ -573,7 +573,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 80, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 6, Sección 2.7 (Valor absoluto) - Ejercicio 38, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 74, Sección 2.2 (Problemas de aplicación) - Ejercicio 35, Sección 2.1 (Ecuaciones) - Ejercicio 13, Sección 2.1 (Ecuaciones) - Ejercicio 67, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 81, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 67, Sección 2.4 (Números complejos) - Ejercicio 57, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 44, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 43, Sección 2.7 (Valor absoluto) - Ejercicio 17, Sección 2.7 (Valor absoluto) - Ejercicio 8, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 55, Sección 2.2 (Problemas de aplicación) - Ejercicio 28, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 68, Sección 2.2 (Problemas de aplicación) - Ejercicio 34, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 62, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 64, Sección 2.7 (Valor absoluto) - Ejercicio 39, Sección 2.1 (Ecuaciones) - Ejercicio 56, Sección 2.2 (Problemas de aplicación) - Ejercicio 1, Sección 2.6 (Desigualdades) - Ejercicio 54, Sección 2.4 (Números complejos) - Ejercicio 24</t>
+          <t>Sección 2.2 (Problemas de aplicación) - Ejercicio 34, Sección 2.6 (Desigualdades) - Ejercicio 21, Sección 2.6 (Desigualdades) - Ejercicio 41, Sección 2.4 (Números complejos) - Ejercicio 44, Sección 2.6 (Desigualdades) - Ejercicio 79, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 54, Sección 2.1 (Ecuaciones) - Ejercicio 45, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 35, Sección 2.6 (Desigualdades) - Ejercicio 87, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 49, Sección 2.1 (Ecuaciones) - Ejercicio 48, Sección 2.6 (Desigualdades) - Ejercicio 51, Sección 2.1 (Ecuaciones) - Ejercicio 24, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 54, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 19, Sección 2.6 (Desigualdades) - Ejercicio 8, Sección 2.4 (Números complejos) - Ejercicio 51, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 61, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 10, Sección 2.2 (Problemas de aplicación) - Ejercicio 15, Sección 2.1 (Ecuaciones) - Ejercicio 5, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 64, Sección 2.6 (Desigualdades) - Ejercicio 56, Sección 2.4 (Números complejos) - Ejercicio 24, Sección 2.6 (Desigualdades) - Ejercicio 9</t>
         </is>
       </c>
     </row>
@@ -585,7 +585,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Sección 2.6 (Desigualdades) - Ejercicio 24, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 39, Sección 2.7 (Valor absoluto) - Ejercicio 16, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 73, Sección 2.4 (Números complejos) - Ejercicio 17, Sección 2.1 (Ecuaciones) - Ejercicio 27, Sección 2.6 (Desigualdades) - Ejercicio 5, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 2, Sección 2.1 (Ecuaciones) - Ejercicio 48, Sección 2.6 (Desigualdades) - Ejercicio 23, Sección 2.2 (Problemas de aplicación) - Ejercicio 9, Sección 2.7 (Valor absoluto) - Ejercicio 10, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 3, Sección 2.2 (Problemas de aplicación) - Ejercicio 32, Sección 2.4 (Números complejos) - Ejercicio 21, Sección 2.6 (Desigualdades) - Ejercicio 71, Sección 2.4 (Números complejos) - Ejercicio 10, Sección 2.1 (Ecuaciones) - Ejercicio 46, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 48, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 47, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 21, Sección 2.1 (Ecuaciones) - Ejercicio 33, Sección 2.4 (Números complejos) - Ejercicio 33, Sección 2.7 (Valor absoluto) - Ejercicio 42, Sección 2.4 (Números complejos) - Ejercicio 40</t>
+          <t>Sección 2.2 (Problemas de aplicación) - Ejercicio 26, Sección 2.4 (Números complejos) - Ejercicio 52, Sección 2.7 (Valor absoluto) - Ejercicio 19, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 4, Sección 2.7 (Valor absoluto) - Ejercicio 17, Sección 2.1 (Ecuaciones) - Ejercicio 78, Sección 2.4 (Números complejos) - Ejercicio 50, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 45, Sección 2.4 (Números complejos) - Ejercicio 43, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 57, Sección 2.1 (Ecuaciones) - Ejercicio 55, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 25, Sección 2.4 (Números complejos) - Ejercicio 31, Sección 2.6 (Desigualdades) - Ejercicio 3, Sección 2.4 (Números complejos) - Ejercicio 39, Sección 2.6 (Desigualdades) - Ejercicio 61, Sección 2.1 (Ecuaciones) - Ejercicio 54, Sección 2.7 (Valor absoluto) - Ejercicio 46, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 62, Sección 2.6 (Desigualdades) - Ejercicio 53, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 46, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 20, Sección 2.4 (Números complejos) - Ejercicio 27, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 78, Sección 2.1 (Ecuaciones) - Ejercicio 64</t>
         </is>
       </c>
     </row>
@@ -597,7 +597,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Sección 2.6 (Desigualdades) - Ejercicio 64, Sección 2.1 (Ecuaciones) - Ejercicio 65, Sección 2.4 (Números complejos) - Ejercicio 36, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 28, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 64, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 31, Sección 2.6 (Desigualdades) - Ejercicio 38, Sección 2.6 (Desigualdades) - Ejercicio 76, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 57, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 37, Sección 2.1 (Ecuaciones) - Ejercicio 57, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 38, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 40, Sección 2.6 (Desigualdades) - Ejercicio 11, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 29, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 25, Sección 2.1 (Ecuaciones) - Ejercicio 32, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 17, Sección 2.1 (Ecuaciones) - Ejercicio 20, Sección 2.2 (Problemas de aplicación) - Ejercicio 26, Sección 2.6 (Desigualdades) - Ejercicio 3, Sección 2.7 (Valor absoluto) - Ejercicio 28, Sección 2.4 (Números complejos) - Ejercicio 43, Sección 2.6 (Desigualdades) - Ejercicio 31, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 59</t>
+          <t>Sección 2.1 (Ecuaciones) - Ejercicio 11, Sección 2.7 (Valor absoluto) - Ejercicio 25, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 31, Sección 2.7 (Valor absoluto) - Ejercicio 43, Sección 2.1 (Ecuaciones) - Ejercicio 70, Sección 2.1 (Ecuaciones) - Ejercicio 49, Sección 2.4 (Números complejos) - Ejercicio 29, Sección 2.6 (Desigualdades) - Ejercicio 88, Sección 2.7 (Valor absoluto) - Ejercicio 39, Sección 2.6 (Desigualdades) - Ejercicio 16, Sección 2.6 (Desigualdades) - Ejercicio 4, Sección 2.1 (Ecuaciones) - Ejercicio 37, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 47, Sección 2.4 (Números complejos) - Ejercicio 48, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 37, Sección 2.7 (Valor absoluto) - Ejercicio 52, Sección 2.7 (Valor absoluto) - Ejercicio 23, Sección 2.1 (Ecuaciones) - Ejercicio 7, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 24, Sección 2.6 (Desigualdades) - Ejercicio 68, Sección 2.2 (Problemas de aplicación) - Ejercicio 16, Sección 2.1 (Ecuaciones) - Ejercicio 63, Sección 2.2 (Problemas de aplicación) - Ejercicio 7, Sección 2.7 (Valor absoluto) - Ejercicio 20, Sección 2.1 (Ecuaciones) - Ejercicio 15</t>
         </is>
       </c>
     </row>
@@ -609,7 +609,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Sección 2.1 (Ecuaciones) - Ejercicio 50, Sección 2.6 (Desigualdades) - Ejercicio 86, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 49, Sección 2.4 (Números complejos) - Ejercicio 29, Sección 2.1 (Ecuaciones) - Ejercicio 28, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 5, Sección 2.1 (Ecuaciones) - Ejercicio 6, Sección 2.4 (Números complejos) - Ejercicio 48, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 69, Sección 2.2 (Problemas de aplicación) - Ejercicio 24, Sección 2.1 (Ecuaciones) - Ejercicio 23, Sección 2.6 (Desigualdades) - Ejercicio 83, Sección 2.1 (Ecuaciones) - Ejercicio 11, Sección 2.7 (Valor absoluto) - Ejercicio 52, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 50, Sección 2.1 (Ecuaciones) - Ejercicio 53, Sección 2.6 (Desigualdades) - Ejercicio 36, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 22, Sección 2.6 (Desigualdades) - Ejercicio 20, Sección 2.4 (Números complejos) - Ejercicio 27, Sección 2.6 (Desigualdades) - Ejercicio 49, Sección 2.7 (Valor absoluto) - Ejercicio 44, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 19, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 58, Sección 2.1 (Ecuaciones) - Ejercicio 8</t>
+          <t>Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 48, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 15, Sección 2.6 (Desigualdades) - Ejercicio 48, Sección 2.4 (Números complejos) - Ejercicio 8, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 69, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 71, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 65, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 20, Sección 2.6 (Desigualdades) - Ejercicio 14, Sección 2.1 (Ecuaciones) - Ejercicio 67, Sección 2.1 (Ecuaciones) - Ejercicio 8, Sección 2.4 (Números complejos) - Ejercicio 30, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 81, Sección 2.2 (Problemas de aplicación) - Ejercicio 24, Sección 2.1 (Ecuaciones) - Ejercicio 60, Sección 2.7 (Valor absoluto) - Ejercicio 35, Sección 2.2 (Problemas de aplicación) - Ejercicio 28, Sección 2.4 (Números complejos) - Ejercicio 58, Sección 2.2 (Problemas de aplicación) - Ejercicio 39, Sección 2.1 (Ecuaciones) - Ejercicio 58, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 51, Sección 2.6 (Desigualdades) - Ejercicio 84, Sección 2.7 (Valor absoluto) - Ejercicio 1, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 67, Sección 2.4 (Números complejos) - Ejercicio 23</t>
         </is>
       </c>
     </row>
@@ -621,7 +621,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Sección 2.4 (Números complejos) - Ejercicio 56, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 47, Sección 2.2 (Problemas de aplicación) - Ejercicio 30, Sección 2.7 (Valor absoluto) - Ejercicio 7, Sección 2.6 (Desigualdades) - Ejercicio 18, Sección 2.2 (Problemas de aplicación) - Ejercicio 14, Sección 2.6 (Desigualdades) - Ejercicio 10, Sección 2.7 (Valor absoluto) - Ejercicio 30, Sección 2.1 (Ecuaciones) - Ejercicio 18, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 14, Sección 2.6 (Desigualdades) - Ejercicio 13, Sección 2.6 (Desigualdades) - Ejercicio 55, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 71, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 62, Sección 2.7 (Valor absoluto) - Ejercicio 32, Sección 2.7 (Valor absoluto) - Ejercicio 15, Sección 2.1 (Ecuaciones) - Ejercicio 22, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 8, Sección 2.7 (Valor absoluto) - Ejercicio 25, Sección 2.6 (Desigualdades) - Ejercicio 19, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 83, Sección 2.4 (Números complejos) - Ejercicio 38, Sección 2.1 (Ecuaciones) - Ejercicio 16, Sección 2.1 (Ecuaciones) - Ejercicio 41, Sección 2.6 (Desigualdades) - Ejercicio 73</t>
+          <t>Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 32, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 47, Sección 2.1 (Ecuaciones) - Ejercicio 19, Sección 2.2 (Problemas de aplicación) - Ejercicio 23, Sección 2.1 (Ecuaciones) - Ejercicio 14, Sección 2.4 (Números complejos) - Ejercicio 41, Sección 2.1 (Ecuaciones) - Ejercicio 51, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 50, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 42, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 29, Sección 2.4 (Números complejos) - Ejercicio 62, Sección 2.4 (Números complejos) - Ejercicio 37, Sección 2.1 (Ecuaciones) - Ejercicio 72, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 9, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 3, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 64, Sección 2.6 (Desigualdades) - Ejercicio 67, Sección 2.2 (Problemas de aplicación) - Ejercicio 18, Sección 2.4 (Números complejos) - Ejercicio 4, Sección 2.1 (Ecuaciones) - Ejercicio 38, Sección 2.1 (Ecuaciones) - Ejercicio 39, Sección 2.4 (Números complejos) - Ejercicio 19, Sección 2.6 (Desigualdades) - Ejercicio 30, Sección 2.1 (Ecuaciones) - Ejercicio 12, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 83</t>
         </is>
       </c>
     </row>
@@ -633,7 +633,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 34, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 41, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 12, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 50, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 54, Sección 2.1 (Ecuaciones) - Ejercicio 31, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 16, Sección 2.4 (Números complejos) - Ejercicio 60, Sección 2.4 (Números complejos) - Ejercicio 25, Sección 2.7 (Valor absoluto) - Ejercicio 13, Sección 2.1 (Ecuaciones) - Ejercicio 10, Sección 2.7 (Valor absoluto) - Ejercicio 14, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 13, Sección 2.4 (Números complejos) - Ejercicio 52, Sección 2.6 (Desigualdades) - Ejercicio 39, Sección 2.2 (Problemas de aplicación) - Ejercicio 8, Sección 2.6 (Desigualdades) - Ejercicio 8, Sección 2.6 (Desigualdades) - Ejercicio 9, Sección 2.6 (Desigualdades) - Ejercicio 57, Sección 2.4 (Números complejos) - Ejercicio 19, Sección 2.2 (Problemas de aplicación) - Ejercicio 40, Sección 2.6 (Desigualdades) - Ejercicio 2, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 14, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 43, Sección 2.6 (Desigualdades) - Ejercicio 35</t>
+          <t>Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 70, Sección 2.1 (Ecuaciones) - Ejercicio 10, Sección 2.7 (Valor absoluto) - Ejercicio 34, Sección 2.2 (Problemas de aplicación) - Ejercicio 12, Sección 2.7 (Valor absoluto) - Ejercicio 36, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 45, Sección 2.6 (Desigualdades) - Ejercicio 66, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 28, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 30, Sección 2.7 (Valor absoluto) - Ejercicio 51, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 68, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 38, Sección 2.7 (Valor absoluto) - Ejercicio 53, Sección 2.1 (Ecuaciones) - Ejercicio 32, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 14, Sección 2.1 (Ecuaciones) - Ejercicio 59, Sección 2.4 (Números complejos) - Ejercicio 60, Sección 2.1 (Ecuaciones) - Ejercicio 47, Sección 2.7 (Valor absoluto) - Ejercicio 30, Sección 2.1 (Ecuaciones) - Ejercicio 69, Sección 2.6 (Desigualdades) - Ejercicio 45, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 66, Sección 2.6 (Desigualdades) - Ejercicio 33, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 19, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 35</t>
         </is>
       </c>
     </row>
@@ -645,7 +645,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Sección 2.6 (Desigualdades) - Ejercicio 43, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 60, Sección 2.7 (Valor absoluto) - Ejercicio 50, Sección 2.1 (Ecuaciones) - Ejercicio 73, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 54, Sección 2.2 (Problemas de aplicación) - Ejercicio 22, Sección 2.6 (Desigualdades) - Ejercicio 87, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 11, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 75, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 76, Sección 2.7 (Valor absoluto) - Ejercicio 4, Sección 2.4 (Números complejos) - Ejercicio 9, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 79, Sección 2.1 (Ecuaciones) - Ejercicio 55, Sección 2.2 (Problemas de aplicación) - Ejercicio 11, Sección 2.7 (Valor absoluto) - Ejercicio 31, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 42, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 45, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 68, Sección 2.2 (Problemas de aplicación) - Ejercicio 29, Sección 2.6 (Desigualdades) - Ejercicio 75, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 52, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 45, Sección 2.4 (Números complejos) - Ejercicio 32, Sección 2.7 (Valor absoluto) - Ejercicio 27</t>
+          <t>Sección 2.6 (Desigualdades) - Ejercicio 28, Sección 2.2 (Problemas de aplicación) - Ejercicio 40, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 5, Sección 2.4 (Números complejos) - Ejercicio 32, Sección 2.4 (Números complejos) - Ejercicio 47, Sección 2.4 (Números complejos) - Ejercicio 13, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 27, Sección 2.6 (Desigualdades) - Ejercicio 6, Sección 2.6 (Desigualdades) - Ejercicio 15, Sección 2.6 (Desigualdades) - Ejercicio 57, Sección 2.1 (Ecuaciones) - Ejercicio 43, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 55, Sección 2.2 (Problemas de aplicación) - Ejercicio 4, Sección 2.4 (Números complejos) - Ejercicio 57, Sección 2.7 (Valor absoluto) - Ejercicio 28, Sección 2.6 (Desigualdades) - Ejercicio 76, Sección 2.1 (Ecuaciones) - Ejercicio 42, Sección 2.7 (Valor absoluto) - Ejercicio 42, Sección 2.4 (Números complejos) - Ejercicio 45, Sección 2.6 (Desigualdades) - Ejercicio 55, Sección 2.6 (Desigualdades) - Ejercicio 32, Sección 2.7 (Valor absoluto) - Ejercicio 7, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 22, Sección 2.1 (Ecuaciones) - Ejercicio 76, Sección 2.1 (Ecuaciones) - Ejercicio 46</t>
         </is>
       </c>
     </row>
@@ -657,7 +657,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Sección 2.2 (Problemas de aplicación) - Ejercicio 7, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 61, Sección 2.6 (Desigualdades) - Ejercicio 60, Sección 2.2 (Problemas de aplicación) - Ejercicio 33, Sección 2.4 (Números complejos) - Ejercicio 4, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 9, Sección 2.6 (Desigualdades) - Ejercicio 32, Sección 2.6 (Desigualdades) - Ejercicio 68, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 33, Sección 2.4 (Números complejos) - Ejercicio 11, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 78, Sección 2.6 (Desigualdades) - Ejercicio 51, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 65, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 6, Sección 2.1 (Ecuaciones) - Ejercicio 30, Sección 2.6 (Desigualdades) - Ejercicio 45, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 13, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 7, Sección 2.6 (Desigualdades) - Ejercicio 33, Sección 2.1 (Ecuaciones) - Ejercicio 38, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 15, Sección 2.6 (Desigualdades) - Ejercicio 67, Sección 2.6 (Desigualdades) - Ejercicio 69, Sección 2.2 (Problemas de aplicación) - Ejercicio 19, Sección 2.6 (Desigualdades) - Ejercicio 16</t>
+          <t>Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 53, Sección 2.6 (Desigualdades) - Ejercicio 18, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 55, Sección 2.1 (Ecuaciones) - Ejercicio 9, Sección 2.6 (Desigualdades) - Ejercicio 36, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 21, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 37, Sección 2.1 (Ecuaciones) - Ejercicio 20, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 14, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 24, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 59, Sección 2.2 (Problemas de aplicación) - Ejercicio 31, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 8, Sección 2.1 (Ecuaciones) - Ejercicio 34, Sección 2.7 (Valor absoluto) - Ejercicio 10, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 34, Sección 2.4 (Números complejos) - Ejercicio 35, Sección 2.4 (Números complejos) - Ejercicio 9, Sección 2.1 (Ecuaciones) - Ejercicio 31, Sección 2.7 (Valor absoluto) - Ejercicio 33, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 18, Sección 2.7 (Valor absoluto) - Ejercicio 41, Sección 2.7 (Valor absoluto) - Ejercicio 54, Sección 2.1 (Ecuaciones) - Ejercicio 61, Sección 2.4 (Números complejos) - Ejercicio 53</t>
         </is>
       </c>
     </row>
@@ -669,7 +669,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 18, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 37, Sección 2.2 (Problemas de aplicación) - Ejercicio 12, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 2, Sección 2.1 (Ecuaciones) - Ejercicio 66, Sección 2.4 (Números complejos) - Ejercicio 59, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 30, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 60, Sección 2.6 (Desigualdades) - Ejercicio 29, Sección 2.7 (Valor absoluto) - Ejercicio 47, Sección 2.2 (Problemas de aplicación) - Ejercicio 25, Sección 2.4 (Números complejos) - Ejercicio 26, Sección 2.1 (Ecuaciones) - Ejercicio 77, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 55, Sección 2.6 (Desigualdades) - Ejercicio 79, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 67, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 22, Sección 2.1 (Ecuaciones) - Ejercicio 61, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 24, Sección 2.6 (Desigualdades) - Ejercicio 6, Sección 2.4 (Números complejos) - Ejercicio 55, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 36, Sección 2.1 (Ecuaciones) - Ejercicio 19, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 7, Sección 2.7 (Valor absoluto) - Ejercicio 46</t>
+          <t>Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 53, Sección 2.2 (Problemas de aplicación) - Ejercicio 10, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 56, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 18, Sección 2.2 (Problemas de aplicación) - Ejercicio 32, Sección 2.7 (Valor absoluto) - Ejercicio 11, Sección 2.1 (Ecuaciones) - Ejercicio 29, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 27, Sección 2.1 (Ecuaciones) - Ejercicio 73, Sección 2.6 (Desigualdades) - Ejercicio 58, Sección 2.4 (Números complejos) - Ejercicio 28, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 7, Sección 2.1 (Ecuaciones) - Ejercicio 53, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 43, Sección 2.7 (Valor absoluto) - Ejercicio 4, Sección 2.4 (Números complejos) - Ejercicio 12, Sección 2.3 (Ecuaciones cuadráticas) - Ejercicio 31, Sección 2.6 (Desigualdades) - Ejercicio 64, Sección 2.1 (Ecuaciones) - Ejercicio 75, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 9, Sección 2.1 (Ecuaciones) - Ejercicio 30, Sección 2.5 (Otros tipos de ecuaciones) - Ejercicio 60, Sección 2.6 (Desigualdades) - Ejercicio 89, Sección 2.7 (Valor absoluto) - Ejercicio 9, Sección 2.1 (Ecuaciones) - Ejercicio 68</t>
         </is>
       </c>
     </row>

</xml_diff>